<commit_message>
Fim da aula 4
</commit_message>
<xml_diff>
--- a/Ficha2/TabelaComCaracteristicasDasClasses.xlsx
+++ b/Ficha2/TabelaComCaracteristicasDasClasses.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escola\Licenciatura\1º Ano\2_Semestre\Programacao_II\Praticas\Ficha2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D000F4B-C5E9-43C5-9FA6-F1F05A13161F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E52C6A9-746D-42FC-BAD3-4B010A8C760A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="30" r:id="rId1"/>
     <sheet name="Ficha1" sheetId="29" r:id="rId2"/>
     <sheet name="Ficha2" sheetId="31" r:id="rId3"/>
+    <sheet name="Ficha3" sheetId="32" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="45">
   <si>
     <t>Atributos</t>
   </si>
@@ -124,6 +125,39 @@
   </si>
   <si>
     <t xml:space="preserve">desassociarProfessor() </t>
+  </si>
+  <si>
+    <t>DiaSemana</t>
+  </si>
+  <si>
+    <t>Enum</t>
+  </si>
+  <si>
+    <t>Horario</t>
+  </si>
+  <si>
+    <t>diasemana</t>
+  </si>
+  <si>
+    <t>hora</t>
+  </si>
+  <si>
+    <t>Int</t>
+  </si>
+  <si>
+    <t>duracao</t>
+  </si>
+  <si>
+    <t>getDiaSemana( )</t>
+  </si>
+  <si>
+    <t>getHora( )</t>
+  </si>
+  <si>
+    <t>getDuracao( )</t>
+  </si>
+  <si>
+    <t>int</t>
   </si>
 </sst>
 </file>
@@ -2828,8 +2862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15747063-0073-4735-83AB-8B474177E0E2}">
   <dimension ref="A1:AD220"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
@@ -4255,4 +4289,1669 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69F28DB9-6219-4186-997C-34627962CA69}">
+  <dimension ref="A1:AD220"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="30" width="3.7109375" style="5" customWidth="1"/>
+    <col min="31" max="16384" width="8.7109375" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="4"/>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+    </row>
+    <row r="2" spans="1:30" ht="95.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+    </row>
+    <row r="3" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="9"/>
+    </row>
+    <row r="4" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="11"/>
+      <c r="AC4" s="11"/>
+      <c r="AD4" s="11"/>
+    </row>
+    <row r="5" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="11"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="11"/>
+      <c r="AB5" s="11"/>
+      <c r="AC5" s="11"/>
+      <c r="AD5" s="11"/>
+    </row>
+    <row r="6" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11"/>
+    </row>
+    <row r="7" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="11"/>
+      <c r="AD7" s="11"/>
+    </row>
+    <row r="8" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="11"/>
+      <c r="AC8" s="11"/>
+      <c r="AD8" s="11"/>
+    </row>
+    <row r="9" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="11"/>
+      <c r="AA9" s="11"/>
+      <c r="AB9" s="11"/>
+      <c r="AC9" s="11"/>
+      <c r="AD9" s="11"/>
+    </row>
+    <row r="10" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="11"/>
+      <c r="AD10" s="11"/>
+    </row>
+    <row r="11" spans="1:30" ht="10.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="11"/>
+      <c r="AD11" s="11"/>
+    </row>
+    <row r="12" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
+      <c r="X12" s="11"/>
+      <c r="Y12" s="11"/>
+      <c r="Z12" s="11"/>
+      <c r="AA12" s="11"/>
+      <c r="AB12" s="11"/>
+      <c r="AC12" s="11"/>
+      <c r="AD12" s="11"/>
+    </row>
+    <row r="13" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="11"/>
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="11"/>
+      <c r="AA13" s="11"/>
+      <c r="AB13" s="11"/>
+      <c r="AC13" s="11"/>
+      <c r="AD13" s="11"/>
+    </row>
+    <row r="14" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="11"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="11"/>
+      <c r="AC14" s="11"/>
+      <c r="AD14" s="11"/>
+    </row>
+    <row r="15" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="11"/>
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="11"/>
+      <c r="AC15" s="11"/>
+      <c r="AD15" s="11"/>
+    </row>
+    <row r="16" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
+      <c r="Y16" s="8"/>
+      <c r="Z16" s="8"/>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="9"/>
+      <c r="AC16" s="9"/>
+      <c r="AD16" s="9"/>
+    </row>
+    <row r="17" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
+      <c r="V17" s="11"/>
+      <c r="W17" s="11"/>
+      <c r="X17" s="11"/>
+      <c r="Y17" s="11"/>
+      <c r="Z17" s="11"/>
+      <c r="AA17" s="11"/>
+      <c r="AB17" s="11"/>
+      <c r="AC17" s="11"/>
+      <c r="AD17" s="11"/>
+    </row>
+    <row r="18" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="11"/>
+      <c r="AC18" s="11"/>
+      <c r="AD18" s="11"/>
+    </row>
+    <row r="19" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+      <c r="X19" s="11"/>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="11"/>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="11"/>
+      <c r="AC19" s="11"/>
+      <c r="AD19" s="11"/>
+    </row>
+    <row r="20" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+      <c r="X20" s="11"/>
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="11"/>
+      <c r="AA20" s="11"/>
+      <c r="AB20" s="11"/>
+      <c r="AC20" s="11"/>
+      <c r="AD20" s="11"/>
+    </row>
+    <row r="21" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+      <c r="X21" s="11"/>
+      <c r="Y21" s="11"/>
+      <c r="Z21" s="11"/>
+      <c r="AA21" s="11"/>
+      <c r="AB21" s="11"/>
+      <c r="AC21" s="11"/>
+      <c r="AD21" s="11"/>
+    </row>
+    <row r="22" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="11"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="11"/>
+      <c r="X22" s="11"/>
+      <c r="Y22" s="11"/>
+      <c r="Z22" s="11"/>
+      <c r="AA22" s="11"/>
+      <c r="AB22" s="11"/>
+      <c r="AC22" s="11"/>
+      <c r="AD22" s="11"/>
+    </row>
+    <row r="23" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+      <c r="V23" s="11"/>
+      <c r="W23" s="11"/>
+      <c r="X23" s="11"/>
+      <c r="Y23" s="11"/>
+      <c r="Z23" s="11"/>
+      <c r="AA23" s="11"/>
+      <c r="AB23" s="11"/>
+      <c r="AC23" s="11"/>
+      <c r="AD23" s="11"/>
+    </row>
+    <row r="24" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11"/>
+      <c r="W24" s="11"/>
+      <c r="X24" s="11"/>
+      <c r="Y24" s="11"/>
+      <c r="Z24" s="11"/>
+      <c r="AA24" s="11"/>
+      <c r="AB24" s="11"/>
+      <c r="AC24" s="11"/>
+      <c r="AD24" s="11"/>
+    </row>
+    <row r="25" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
+      <c r="V25" s="11"/>
+      <c r="W25" s="11"/>
+      <c r="X25" s="11"/>
+      <c r="Y25" s="11"/>
+      <c r="Z25" s="11"/>
+      <c r="AA25" s="11"/>
+      <c r="AB25" s="11"/>
+      <c r="AC25" s="11"/>
+      <c r="AD25" s="11"/>
+    </row>
+    <row r="26" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11"/>
+      <c r="V26" s="11"/>
+      <c r="W26" s="11"/>
+      <c r="X26" s="11"/>
+      <c r="Y26" s="11"/>
+      <c r="Z26" s="11"/>
+      <c r="AA26" s="11"/>
+      <c r="AB26" s="11"/>
+      <c r="AC26" s="11"/>
+      <c r="AD26" s="11"/>
+    </row>
+    <row r="27" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+      <c r="T27" s="11"/>
+      <c r="U27" s="11"/>
+      <c r="V27" s="11"/>
+      <c r="W27" s="11"/>
+      <c r="X27" s="11"/>
+      <c r="Y27" s="11"/>
+      <c r="Z27" s="11"/>
+      <c r="AA27" s="11"/>
+      <c r="AB27" s="11"/>
+      <c r="AC27" s="11"/>
+      <c r="AD27" s="11"/>
+    </row>
+    <row r="28" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+      <c r="V28" s="11"/>
+      <c r="W28" s="11"/>
+      <c r="X28" s="11"/>
+      <c r="Y28" s="11"/>
+      <c r="Z28" s="11"/>
+      <c r="AA28" s="11"/>
+      <c r="AB28" s="11"/>
+      <c r="AC28" s="11"/>
+      <c r="AD28" s="11"/>
+    </row>
+    <row r="29" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
+      <c r="T29" s="11"/>
+      <c r="U29" s="11"/>
+      <c r="V29" s="11"/>
+      <c r="W29" s="11"/>
+      <c r="X29" s="11"/>
+      <c r="Y29" s="11"/>
+      <c r="Z29" s="11"/>
+      <c r="AA29" s="11"/>
+      <c r="AB29" s="11"/>
+      <c r="AC29" s="11"/>
+      <c r="AD29" s="11"/>
+    </row>
+    <row r="30" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
+      <c r="U30" s="11"/>
+      <c r="V30" s="11"/>
+      <c r="W30" s="11"/>
+      <c r="X30" s="11"/>
+      <c r="Y30" s="11"/>
+      <c r="Z30" s="11"/>
+      <c r="AA30" s="11"/>
+      <c r="AB30" s="11"/>
+      <c r="AC30" s="11"/>
+      <c r="AD30" s="11"/>
+    </row>
+    <row r="31" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
+      <c r="T31" s="11"/>
+      <c r="U31" s="11"/>
+      <c r="V31" s="11"/>
+      <c r="W31" s="11"/>
+      <c r="X31" s="11"/>
+      <c r="Y31" s="11"/>
+      <c r="Z31" s="11"/>
+      <c r="AA31" s="11"/>
+      <c r="AB31" s="11"/>
+      <c r="AC31" s="11"/>
+      <c r="AD31" s="11"/>
+    </row>
+    <row r="32" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+      <c r="T32" s="11"/>
+      <c r="U32" s="11"/>
+      <c r="V32" s="11"/>
+      <c r="W32" s="11"/>
+      <c r="X32" s="11"/>
+      <c r="Y32" s="11"/>
+      <c r="Z32" s="11"/>
+      <c r="AA32" s="11"/>
+      <c r="AB32" s="11"/>
+      <c r="AC32" s="11"/>
+      <c r="AD32" s="11"/>
+    </row>
+    <row r="33" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="11"/>
+      <c r="T33" s="11"/>
+      <c r="U33" s="11"/>
+      <c r="V33" s="11"/>
+      <c r="W33" s="11"/>
+      <c r="X33" s="11"/>
+      <c r="Y33" s="11"/>
+      <c r="Z33" s="11"/>
+      <c r="AA33" s="11"/>
+      <c r="AB33" s="11"/>
+      <c r="AC33" s="11"/>
+      <c r="AD33" s="11"/>
+    </row>
+    <row r="34" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="11"/>
+      <c r="T34" s="11"/>
+      <c r="U34" s="11"/>
+      <c r="V34" s="11"/>
+      <c r="W34" s="11"/>
+      <c r="X34" s="11"/>
+      <c r="Y34" s="11"/>
+      <c r="Z34" s="11"/>
+      <c r="AA34" s="11"/>
+      <c r="AB34" s="11"/>
+      <c r="AC34" s="11"/>
+      <c r="AD34" s="11"/>
+    </row>
+    <row r="35" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="11"/>
+      <c r="T35" s="11"/>
+      <c r="U35" s="11"/>
+      <c r="V35" s="11"/>
+      <c r="W35" s="11"/>
+      <c r="X35" s="11"/>
+      <c r="Y35" s="11"/>
+      <c r="Z35" s="11"/>
+      <c r="AA35" s="11"/>
+      <c r="AB35" s="11"/>
+      <c r="AC35" s="11"/>
+      <c r="AD35" s="11"/>
+    </row>
+    <row r="36" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11"/>
+      <c r="T36" s="11"/>
+      <c r="U36" s="11"/>
+      <c r="V36" s="11"/>
+      <c r="W36" s="11"/>
+      <c r="X36" s="11"/>
+      <c r="Y36" s="11"/>
+      <c r="Z36" s="11"/>
+      <c r="AA36" s="11"/>
+      <c r="AB36" s="11"/>
+      <c r="AC36" s="11"/>
+      <c r="AD36" s="11"/>
+    </row>
+    <row r="37" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="11"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="11"/>
+      <c r="T37" s="11"/>
+      <c r="U37" s="11"/>
+      <c r="V37" s="11"/>
+      <c r="W37" s="11"/>
+      <c r="X37" s="11"/>
+      <c r="Y37" s="11"/>
+      <c r="Z37" s="11"/>
+      <c r="AA37" s="11"/>
+      <c r="AB37" s="11"/>
+      <c r="AC37" s="11"/>
+      <c r="AD37" s="11"/>
+    </row>
+    <row r="38" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
+      <c r="M38" s="11"/>
+      <c r="N38" s="11"/>
+      <c r="O38" s="11"/>
+      <c r="P38" s="11"/>
+      <c r="Q38" s="11"/>
+      <c r="R38" s="11"/>
+      <c r="S38" s="11"/>
+      <c r="T38" s="11"/>
+      <c r="U38" s="11"/>
+      <c r="V38" s="11"/>
+      <c r="W38" s="11"/>
+      <c r="X38" s="11"/>
+      <c r="Y38" s="11"/>
+      <c r="Z38" s="11"/>
+      <c r="AA38" s="11"/>
+      <c r="AB38" s="11"/>
+      <c r="AC38" s="11"/>
+      <c r="AD38" s="11"/>
+    </row>
+    <row r="39" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11"/>
+      <c r="O39" s="11"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="11"/>
+      <c r="S39" s="11"/>
+      <c r="T39" s="11"/>
+      <c r="U39" s="11"/>
+      <c r="V39" s="11"/>
+      <c r="W39" s="11"/>
+      <c r="X39" s="11"/>
+      <c r="Y39" s="11"/>
+      <c r="Z39" s="11"/>
+      <c r="AA39" s="11"/>
+      <c r="AB39" s="11"/>
+      <c r="AC39" s="11"/>
+      <c r="AD39" s="11"/>
+    </row>
+    <row r="40" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="137" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="138" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="139" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="140" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="142" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="143" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="145" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="146" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="148" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="149" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="150" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="151" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="152" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="153" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="154" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="155" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="156" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="157" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="158" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="160" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="161" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="162" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="163" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="164" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="166" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="174" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="175" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="176" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="177" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="178" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="179" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="180" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="181" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="182" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="183" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="184" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="185" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="186" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="187" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="188" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="189" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="190" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="191" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="192" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="193" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="194" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="195" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="196" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="197" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="198" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="199" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="200" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="201" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="202" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="203" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="204" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="205" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="206" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="207" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="208" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="209" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="210" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="211" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="212" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="213" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="214" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="215" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="216" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="217" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="218" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="219" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="220" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final da aula 4
</commit_message>
<xml_diff>
--- a/Ficha2/TabelaComCaracteristicasDasClasses.xlsx
+++ b/Ficha2/TabelaComCaracteristicasDasClasses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escola\Licenciatura\1º Ano\2_Semestre\Programacao_II\Praticas\Ficha2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E52C6A9-746D-42FC-BAD3-4B010A8C760A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1F87F5-9601-4248-967D-A202D0A72753}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="2760" windowWidth="21600" windowHeight="11385" tabRatio="903" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="30" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="49">
   <si>
     <t>Atributos</t>
   </si>
@@ -151,13 +151,25 @@
     <t>getDiaSemana( )</t>
   </si>
   <si>
-    <t>getHora( )</t>
-  </si>
-  <si>
     <t>getDuracao( )</t>
   </si>
   <si>
     <t>int</t>
+  </si>
+  <si>
+    <t>getHorarios( )</t>
+  </si>
+  <si>
+    <t>horainicio</t>
+  </si>
+  <si>
+    <t>getAulas( )</t>
+  </si>
+  <si>
+    <t>getAulas(Horario)</t>
+  </si>
+  <si>
+    <t>getHoraInicio( )</t>
   </si>
 </sst>
 </file>
@@ -4296,10 +4308,10 @@
   <dimension ref="A1:AD220"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
+      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4781,11 +4793,17 @@
       <c r="AD12" s="11"/>
     </row>
     <row r="13" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
+      <c r="A13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
+      <c r="E13" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
@@ -5502,10 +5520,10 @@
     </row>
     <row r="32" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
@@ -5540,10 +5558,10 @@
     </row>
     <row r="33" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
@@ -5577,11 +5595,17 @@
       <c r="AD33" s="11"/>
     </row>
     <row r="34" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
+      <c r="A34" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>44</v>
+      </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
+      <c r="E34" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
       <c r="H34" s="11"/>
@@ -5609,10 +5633,18 @@
       <c r="AD34" s="11"/>
     </row>
     <row r="35" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="10"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
+      <c r="A35" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
@@ -5641,10 +5673,18 @@
       <c r="AD35" s="11"/>
     </row>
     <row r="36" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="10"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
+      <c r="A36" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>

</xml_diff>